<commit_message>
process 2021 underwater data; started 2021 weather data
</commit_message>
<xml_diff>
--- a/AubBuoy_FlagCodeDefinitions.xlsx
+++ b/AubBuoy_FlagCodeDefinitions.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>errant code</t>
-  </si>
-  <si>
-    <t>&lt;-99999</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>flag</t>
   </si>
@@ -41,22 +32,28 @@
     <t>description</t>
   </si>
   <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>per datetimestamp range</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>buoy maintenance</t>
-  </si>
-  <si>
-    <t>includes deployment</t>
-  </si>
-  <si>
-    <t>notes</t>
+    <t>w</t>
+  </si>
+  <si>
+    <t>do sensor cleaned</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>weather station adjusted to orient more northward</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>removed buoy</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>buoy deployed for season</t>
   </si>
 </sst>
 </file>
@@ -374,53 +371,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021 data cleaning complete
</commit_message>
<xml_diff>
--- a/AubBuoy_FlagCodeDefinitions.xlsx
+++ b/AubBuoy_FlagCodeDefinitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steeleb\Dropbox\Lake Auburn Buoy\programs\Auburn_buoy_data_cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steeleb\Dropbox\Lake Auburn Buoy\programs\Auburn_buoy_GH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>flag</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>buoy deployed for season</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>rain gague malfunction; values incorrect - recoded to na</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>data errant, recoded to na</t>
   </si>
 </sst>
 </file>
@@ -371,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -422,6 +434,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add flags to 2013
</commit_message>
<xml_diff>
--- a/AubBuoy_FlagCodeDefinitions.xlsx
+++ b/AubBuoy_FlagCodeDefinitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>flag</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>data errant, recoded to na</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>data reporting intermittently</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>do sensor calibrated</t>
+  </si>
+  <si>
+    <t>flag_temp</t>
+  </si>
+  <si>
+    <t>flag_do</t>
+  </si>
+  <si>
+    <t>flag_met</t>
   </si>
 </sst>
 </file>
@@ -383,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -404,50 +425,81 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021 - updated rain calcs and fixed datetime DST issue
</commit_message>
<xml_diff>
--- a/AubBuoy_FlagCodeDefinitions.xlsx
+++ b/AubBuoy_FlagCodeDefinitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>flag</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>flag_met</t>
+  </si>
+  <si>
+    <t>presumed calibrated</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>sensor replaced (prefaced by depth of sensor)</t>
+  </si>
+  <si>
+    <t>sensor replaced</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>sensor failed</t>
+  </si>
+  <si>
+    <t>precip values interpolated (linear) from adjacent records</t>
   </si>
 </sst>
 </file>
@@ -404,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -460,46 +484,86 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>19</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add s & e defs
</commit_message>
<xml_diff>
--- a/AubBuoy_FlagCodeDefinitions.xlsx
+++ b/AubBuoy_FlagCodeDefinitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steeleb\Dropbox\Lake Auburn Buoy\programs\Auburn_buoy_GH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steeleb\Documents\GitHub\Auburn_buoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>flag</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>precip values interpolated (linear) from adjacent records</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>suspect behavior, use with caution</t>
+  </si>
+  <si>
+    <t>data errant, recoded to NA</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -537,32 +546,48 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>